<commit_message>
Fixes for race condition
</commit_message>
<xml_diff>
--- a/Arduino/Apps/Bumblebee_Displacement_Detector/Displacement Detector Writeup/Misc.xlsx
+++ b/Arduino/Apps/Bumblebee_Displacement_Detector/Displacement Detector Writeup/Misc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>I</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Deg</t>
   </si>
   <si>
-    <t>Prev</t>
-  </si>
-  <si>
     <t>Mult</t>
   </si>
   <si>
@@ -41,6 +38,21 @@
   </si>
   <si>
     <t>C2</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>LHS</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>counterclockwise</t>
+  </si>
+  <si>
+    <t>clockwise</t>
   </si>
 </sst>
 </file>
@@ -50,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +71,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -74,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -82,17 +102,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -398,15 +446,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A8" sqref="A8:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="3.109375" style="4" customWidth="1"/>
+    <col min="2" max="3" width="2.6640625" customWidth="1"/>
+    <col min="4" max="4" width="4.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -423,12 +474,12 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
+      <c r="A2" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -446,8 +497,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
+      <c r="A3" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B3">
         <v>-1</v>
@@ -469,8 +520,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
+      <c r="A4" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -492,8 +543,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
+      <c r="A5" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B5">
         <v>-3</v>
@@ -514,7 +565,98 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8">
+        <f>C2</f>
+        <v>2</v>
+      </c>
+      <c r="C9" s="8">
+        <f>B2</f>
+        <v>4</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="8">
+        <f t="shared" ref="B10:B12" si="0">C3</f>
+        <v>3</v>
+      </c>
+      <c r="C10" s="8">
+        <f t="shared" ref="C10:C12" si="1">B3</f>
+        <v>-1</v>
+      </c>
+      <c r="D10" s="8">
+        <f>F3</f>
+        <v>14</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="C11" s="8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D11" s="8">
+        <f>F4</f>
+        <v>-10</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="C12" s="8">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+      <c r="D12" s="8">
+        <f>F5</f>
+        <v>2</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>